<commit_message>
Initial pDC expression analysis
</commit_message>
<xml_diff>
--- a/Single-cell_BPDCN_colors.xlsx
+++ b/Single-cell_BPDCN_colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/Github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2614D0AF-57E8-BF49-90D9-52C34B5CC898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD7AA47-0B0E-9143-AF53-8823BBAC4569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{BA969524-A657-654B-876F-EEF4C1226972}"/>
+    <workbookView xWindow="8360" yWindow="760" windowWidth="26200" windowHeight="21580" xr2:uid="{BA969524-A657-654B-876F-EEF4C1226972}"/>
   </bookViews>
   <sheets>
     <sheet name="BPDCN" sheetId="2" r:id="rId1"/>
@@ -472,15 +472,6 @@
     <t>#dc143c</t>
   </si>
   <si>
-    <t>no_call</t>
-  </si>
-  <si>
-    <t>Grey</t>
-  </si>
-  <si>
-    <t>#808080</t>
-  </si>
-  <si>
     <t>healthy_bm</t>
   </si>
   <si>
@@ -506,13 +497,22 @@
   </si>
   <si>
     <t>Tomato</t>
+  </si>
+  <si>
+    <t>Gainsboro</t>
+  </si>
+  <si>
+    <t>#dcdcdc</t>
+  </si>
+  <si>
+    <t>no call</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -547,8 +547,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="60">
+  <fills count="56">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,12 +564,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF012BE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF2A4BD7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -731,18 +732,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA52A2A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8C00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFD700"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -773,12 +762,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4B0092"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF8FBC8F"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -881,12 +864,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00FF7F"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -900,6 +877,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6347"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCDCDC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,8 +908,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -934,14 +918,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
@@ -954,60 +938,57 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="52" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="53" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="53" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="54" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="56" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="57" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="59" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="54" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,6 +997,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDCDCDC"/>
       <color rgb="FFFF6347"/>
       <color rgb="FF4682B4"/>
       <color rgb="FF00FF7F"/>
@@ -1025,7 +1007,6 @@
       <color rgb="FF00CED1"/>
       <color rgb="FF00BFFF"/>
       <color rgb="FFF08080"/>
-      <color rgb="FFDDA0DD"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1339,7 +1320,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1525,19 +1506,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="45" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
+    <row r="18" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="44" t="s">
         <v>114</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1547,19 +1528,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+    <row r="19" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="43" t="s">
         <v>112</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1569,52 +1550,52 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="50" t="s">
+    <row r="21" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="46" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="52" t="s">
+    <row r="22" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
         <v>122</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="53" t="s">
+    <row r="23" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="49" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55" t="s">
+    <row r="24" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="51" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="42" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="29" t="s">
@@ -1625,7 +1606,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="59" t="s">
         <v>129</v>
       </c>
       <c r="B26" s="28" t="s">
@@ -1636,310 +1617,310 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="58" t="s">
+      <c r="A27" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="56" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="58" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="65" t="s">
+      <c r="B29" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="61" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="63" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="69" t="s">
+      <c r="C31" s="65" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="34" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="36" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="37" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="38" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="39" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="40" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="52" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="48" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="53" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="73" t="s">
+    <row r="43" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="68" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="73" t="s">
+      <c r="C43" s="68" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="73" t="s">
+    </row>
+    <row r="45" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="B45" s="72" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="B44" s="75" t="s">
+      <c r="C45" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="76" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" s="67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" s="73" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="77" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="77" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" s="77" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="C46" s="70" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="71" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" s="71" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="72" t="s">
-        <v>145</v>
-      </c>
-      <c r="B48" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" s="72" t="s">
-        <v>146</v>
-      </c>
-    </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="74" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="33" t="s">
+      <c r="B50" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="74" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="33" t="s">
+      <c r="A51" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C51" s="74" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="74" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="74" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="75" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reclassify and hierarchy plots (v1)
Add folder 10_Hierarchy and other minor updates.
</commit_message>
<xml_diff>
--- a/Single-cell_BPDCN_colors.xlsx
+++ b/Single-cell_BPDCN_colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/Github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/scBPDCN-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1F0CDA-73F5-294D-A413-BFBD365E60B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE56DB-DE7F-3A44-9599-B5972F057880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{BA969524-A657-654B-876F-EEF4C1226972}"/>
+    <workbookView xWindow="6740" yWindow="1440" windowWidth="17280" windowHeight="21580" xr2:uid="{BA969524-A657-654B-876F-EEF4C1226972}"/>
   </bookViews>
   <sheets>
     <sheet name="BPDCN" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
   <si>
     <t>pop</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Plasma</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>NK</t>
@@ -1282,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583C9BB9-9230-124C-8443-57AE6702EAE7}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,54 +1297,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1355,10 +1352,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1366,21 +1363,21 @@
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1388,10 +1385,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1399,10 +1396,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1410,21 +1407,21 @@
         <v>5</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1432,10 +1429,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1443,384 +1440,373 @@
         <v>7</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="32" t="s">
+    </row>
+    <row r="23" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="59" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="71" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="71" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="73" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B42" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="62" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="66" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="B27" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" s="52" t="s">
-        <v>114</v>
-      </c>
-      <c r="C28" s="52" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="B29" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" s="55" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" s="57" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="59" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="B33" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="C33" s="71" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="C36" s="73" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="74" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="74" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="70" t="s">
-        <v>133</v>
-      </c>
-      <c r="C38" s="70" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="B41" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C41" s="69" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="B42" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="68" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" s="62" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="63" t="s">
-        <v>142</v>
-      </c>
-      <c r="B44" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="65" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="66" t="s">
-        <v>141</v>
-      </c>
-      <c r="B45" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="66" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="67" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C47" s="61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="67" t="s">
-        <v>129</v>
-      </c>
-      <c r="B48" s="67" t="s">
-        <v>128</v>
-      </c>
-      <c r="C48" s="67" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1842,57 +1828,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Streamlined all downstream analysis
Gene expression, healthy / premalignant / malignant classification, integration of  mutation data.
</commit_message>
<xml_diff>
--- a/Single-cell_BPDCN_colors.xlsx
+++ b/Single-cell_BPDCN_colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/scBPDCN-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE56DB-DE7F-3A44-9599-B5972F057880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D676CB53-6A7B-784F-B79A-7B75E67989CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="1440" windowWidth="17280" windowHeight="21580" xr2:uid="{BA969524-A657-654B-876F-EEF4C1226972}"/>
+    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{BA969524-A657-654B-876F-EEF4C1226972}"/>
   </bookViews>
   <sheets>
     <sheet name="BPDCN" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="156">
   <si>
     <t>pop</t>
   </si>
@@ -470,6 +470,39 @@
   </si>
   <si>
     <t>#ffa07a</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>Premalignant</t>
+  </si>
+  <si>
+    <t>Malignant</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>#bdb76b</t>
+  </si>
+  <si>
+    <t>#ff69b4</t>
+  </si>
+  <si>
+    <t>#b22222</t>
+  </si>
+  <si>
+    <t>#d3d3d3</t>
+  </si>
+  <si>
+    <t>LightGrey</t>
+  </si>
+  <si>
+    <t>FireBrick</t>
+  </si>
+  <si>
+    <t>DarkKhaki</t>
   </si>
 </sst>
 </file>
@@ -512,7 +545,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="57">
+  <fills count="60">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +879,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDA70D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDB76B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB22222"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3D3D3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -951,6 +1002,10 @@
     <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,16 +1014,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD3D3D3"/>
+      <color rgb="FFB22222"/>
+      <color rgb="FFFF69B4"/>
+      <color rgb="FFBDB76B"/>
       <color rgb="FFFFA07A"/>
       <color rgb="FFDA70D6"/>
       <color rgb="FFDDA0DD"/>
       <color rgb="FF8FBC8F"/>
       <color rgb="FFA0522D"/>
       <color rgb="FFFFD700"/>
-      <color rgb="FFBC8F8F"/>
-      <color rgb="FFF0E68C"/>
-      <color rgb="FF6A5ACD"/>
-      <color rgb="FFFF69B4"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1279,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583C9BB9-9230-124C-8443-57AE6702EAE7}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1807,6 +1862,50 @@
       </c>
       <c r="C47" s="67" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" s="75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B50" s="77" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="77" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="78" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="78" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>